<commit_message>
Einführung, Theorie und Ergebnisse Daten
</commit_message>
<xml_diff>
--- a/02_Versuch SURF/data/data.xlsx
+++ b/02_Versuch SURF/data/data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Desktop\Studium\4. Semester\PC2_Protokolle\02_Versuch SURF\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Studium\PC2_Protokolle\02_Versuch SURF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EFC516-9E81-47E3-9041-AACAA06E22FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5D55DC-80D1-4943-B0DA-A28489E3CEDC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{09E9FFC4-CFD6-4C29-84B8-7DE51913CD17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{09E9FFC4-CFD6-4C29-84B8-7DE51913CD17}"/>
   </bookViews>
   <sheets>
     <sheet name="Temperaturabhängigkeit" sheetId="2" r:id="rId1"/>
     <sheet name="Daten SURF" sheetId="1" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="5" r:id="rId3"/>
+    <sheet name="Tabelle2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
     <t>T in °C</t>
   </si>
@@ -113,13 +113,41 @@
   <si>
     <t>Ausreißer -</t>
   </si>
+  <si>
+    <t>K ethanol</t>
+  </si>
+  <si>
+    <t>K Nacl</t>
+  </si>
+  <si>
+    <t>K NaDDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NaCl korr </t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Stoff</t>
+  </si>
+  <si>
+    <t>Dichtefaktor</t>
+  </si>
+  <si>
+    <t>Oberflächenspannung gemessen</t>
+  </si>
+  <si>
+    <t>Sigma korr</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -246,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -258,9 +286,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -269,11 +297,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -557,7 +612,7 @@
           </c:marker>
           <c:trendline>
             <c:spPr>
-              <a:ln w="28575" cap="rnd">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
@@ -569,12 +624,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.2911502371495517E-2"/>
-                  <c:y val="2.7064349530165167E-2"/>
-                </c:manualLayout>
-              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -600,7 +649,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -726,7 +775,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="724987903"/>
@@ -788,7 +837,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="83456031"/>
@@ -836,7 +885,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1402,7 +1451,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{73E6AD21-8903-4C98-A116-50844A271990}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1413,7 +1462,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6011155"/>
+    <xdr:ext cx="9290137" cy="6002055"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -1739,18 +1788,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64ADF54-4F62-4412-A23F-893180B0009B}">
-  <dimension ref="B1:T26"/>
+  <dimension ref="B1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="K14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="W42" sqref="W42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30" customWidth="1"/>
     <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1918,7 +1970,7 @@
         <v>69</v>
       </c>
       <c r="T5" s="14">
-        <f t="shared" ref="T5:T8" si="3">P5-Q5*3</f>
+        <f t="shared" ref="T5" si="3">P5-Q5*3</f>
         <v>69</v>
       </c>
     </row>
@@ -2064,7 +2116,8 @@
         <v>1</v>
       </c>
       <c r="H9" s="11">
-        <v>66.099999999999994</v>
+        <f>66.1*$C$23</f>
+        <v>68.80297397769516</v>
       </c>
       <c r="I9" s="11">
         <v>65</v>
@@ -2427,7 +2480,7 @@
       </c>
       <c r="H19" s="11">
         <f>AVERAGE(H9:H18)</f>
-        <v>67.98</v>
+        <v>68.250297397769515</v>
       </c>
       <c r="I19" s="11">
         <f>AVERAGE(I9:I18)</f>
@@ -2466,7 +2519,7 @@
       </c>
       <c r="H20" s="4">
         <f>_xlfn.STDEV.S(H9:H18)</f>
-        <v>0.70047602861673208</v>
+        <v>0.30336617689475753</v>
       </c>
       <c r="I20" s="4">
         <f>_xlfn.STDEV.S(I9:I18)</f>
@@ -2505,7 +2558,7 @@
       </c>
       <c r="H21" s="11">
         <f>H19+3*H20</f>
-        <v>70.081428085850206</v>
+        <v>69.160395928453781</v>
       </c>
       <c r="I21" s="11">
         <f t="shared" ref="I21:J21" si="5">I19+3*I20</f>
@@ -2544,7 +2597,7 @@
       </c>
       <c r="H22" s="11">
         <f>H19-3*H20</f>
-        <v>65.878571914149802</v>
+        <v>67.340198867085249</v>
       </c>
       <c r="I22" s="11">
         <f t="shared" ref="I22:J22" si="6">I19-3*I20</f>
@@ -2583,7 +2636,7 @@
       </c>
       <c r="H23" s="7">
         <f>H20/H19*100</f>
-        <v>1.0304148699863667</v>
+        <v>0.44449063002130135</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" ref="I23:J23" si="7">I20/I19*100</f>
@@ -2607,7 +2660,7 @@
       <c r="S23" s="4"/>
       <c r="T23" s="5"/>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L24" s="3">
         <v>49</v>
       </c>
@@ -2622,7 +2675,13 @@
       <c r="S24" s="4"/>
       <c r="T24" s="5"/>
     </row>
-    <row r="25" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="2"/>
       <c r="L25" s="6">
         <v>49</v>
       </c>
@@ -2637,7 +2696,19 @@
       <c r="S25" s="7"/>
       <c r="T25" s="8"/>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -2646,11 +2717,1585 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
+    <row r="27" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>0.99450000000000005</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="11">
+        <f>H9*$C$23*$C$27</f>
+        <v>71.222587858100354</v>
+      </c>
+      <c r="I27" s="11">
+        <f>I9*$C$23*$C$28</f>
+        <v>68.063940520446096</v>
+      </c>
+      <c r="J27" s="11">
+        <f>J9*$C$23*$C$29</f>
+        <v>38.727434944237913</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="2"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>1.006</v>
+      </c>
+      <c r="G28" s="3">
+        <f>G27+1</f>
+        <v>2</v>
+      </c>
+      <c r="H28" s="11">
+        <f t="shared" ref="H28:H36" si="8">H10*$C$23*$C$27</f>
+        <v>70.391375464684018</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" ref="I28:I36" si="9">I10*$C$23*$C$28</f>
+        <v>67.540371747211893</v>
+      </c>
+      <c r="J28" s="11">
+        <f t="shared" ref="J28:J36" si="10">J10*$C$23*$C$29</f>
+        <v>39.720446096654271</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="R28" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="S28" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="T28" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f>0.954</f>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" ref="G29:G36" si="11">G28+1</f>
+        <v>3</v>
+      </c>
+      <c r="H29" s="11">
+        <f t="shared" si="8"/>
+        <v>70.908959107806695</v>
+      </c>
+      <c r="I29" s="11">
+        <f t="shared" si="9"/>
+        <v>67.435657992565055</v>
+      </c>
+      <c r="J29" s="11">
+        <f t="shared" si="10"/>
+        <v>40.514855018587355</v>
+      </c>
+      <c r="L29" s="3">
+        <v>20</v>
+      </c>
+      <c r="M29" s="20">
+        <f>M4*$C$23</f>
+        <v>72.6542750929368</v>
+      </c>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4">
+        <v>20</v>
+      </c>
+      <c r="P29" s="4">
+        <f>AVERAGE(M29:M38)</f>
+        <v>72.8</v>
+      </c>
+      <c r="Q29" s="20">
+        <f>_xlfn.STDEV.S(M29:M38)</f>
+        <v>8.777573678782484E-2</v>
+      </c>
+      <c r="R29" s="22">
+        <f>Q29/P29*100</f>
+        <v>0.12057106701624293</v>
+      </c>
+      <c r="S29" s="20">
+        <f>P29+Q29*3</f>
+        <v>73.063327210363468</v>
+      </c>
+      <c r="T29" s="14">
+        <f>P29-Q29*3</f>
+        <v>72.536672789636526</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G30" s="3">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="H30" s="11">
+        <f t="shared" si="8"/>
+        <v>70.494892193308544</v>
+      </c>
+      <c r="I30" s="11">
+        <f t="shared" si="9"/>
+        <v>66.493234200743501</v>
+      </c>
+      <c r="J30" s="11">
+        <f t="shared" si="10"/>
+        <v>40.713457249070629</v>
+      </c>
+      <c r="L30" s="3">
+        <v>20</v>
+      </c>
+      <c r="M30" s="20">
+        <f t="shared" ref="M30:M50" si="12">M5*$C$23</f>
+        <v>72.6542750929368</v>
+      </c>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4">
+        <f>L39</f>
+        <v>30</v>
+      </c>
+      <c r="P30" s="20">
+        <f>AVERAGE(M39:M41)</f>
+        <v>71.821561338289968</v>
+      </c>
+      <c r="Q30" s="20">
+        <f>_xlfn.STDEV.S(M39:M41)</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="22">
+        <f t="shared" ref="R30:R33" si="13">Q30/P30*100</f>
+        <v>0</v>
+      </c>
+      <c r="S30" s="20">
+        <f t="shared" ref="S30:S33" si="14">P30+Q30*3</f>
+        <v>71.821561338289968</v>
+      </c>
+      <c r="T30" s="14">
+        <f t="shared" ref="T30" si="15">P30-Q30*3</f>
+        <v>71.821561338289968</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G31" s="3">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="H31" s="11">
+        <f t="shared" si="8"/>
+        <v>70.908959107806695</v>
+      </c>
+      <c r="I31" s="11">
+        <f t="shared" si="9"/>
+        <v>67.540371747211893</v>
+      </c>
+      <c r="J31" s="11">
+        <f t="shared" si="10"/>
+        <v>40.514855018587355</v>
+      </c>
+      <c r="L31" s="3">
+        <v>20</v>
+      </c>
+      <c r="M31" s="20">
+        <f t="shared" si="12"/>
+        <v>72.758364312267659</v>
+      </c>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4">
+        <f>L42</f>
+        <v>35</v>
+      </c>
+      <c r="P31" s="20">
+        <f>AVERAGE(M42:M44)</f>
+        <v>71.162329615861211</v>
+      </c>
+      <c r="Q31" s="20">
+        <f>_xlfn.STDEV.S(M42:M44)</f>
+        <v>0.15899890887083501</v>
+      </c>
+      <c r="R31" s="22">
+        <f t="shared" si="13"/>
+        <v>0.22343128693105083</v>
+      </c>
+      <c r="S31" s="20">
+        <f t="shared" si="14"/>
+        <v>71.639326342473709</v>
+      </c>
+      <c r="T31" s="14">
+        <f>P31-Q31*3</f>
+        <v>70.685332889248713</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G32" s="3">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="H32" s="11">
+        <f t="shared" si="8"/>
+        <v>70.391375464684018</v>
+      </c>
+      <c r="I32" s="11">
+        <f t="shared" si="9"/>
+        <v>67.64508550185873</v>
+      </c>
+      <c r="J32" s="11">
+        <f t="shared" si="10"/>
+        <v>40.713457249070629</v>
+      </c>
+      <c r="L32" s="3">
+        <v>20</v>
+      </c>
+      <c r="M32" s="20">
+        <f t="shared" si="12"/>
+        <v>72.758364312267659</v>
+      </c>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4">
+        <f>L45</f>
+        <v>40</v>
+      </c>
+      <c r="P32" s="20">
+        <f>AVERAGE(M45:M47)</f>
+        <v>70.641883519206942</v>
+      </c>
+      <c r="Q32" s="20">
+        <f>_xlfn.STDEV.S(M45:M47)</f>
+        <v>0.12019187760081929</v>
+      </c>
+      <c r="R32" s="22">
+        <f t="shared" si="13"/>
+        <v>0.17014251547828579</v>
+      </c>
+      <c r="S32" s="20">
+        <f t="shared" si="14"/>
+        <v>71.002459152009394</v>
+      </c>
+      <c r="T32" s="14">
+        <f>P32-Q32*3</f>
+        <v>70.281307886404491</v>
+      </c>
+    </row>
+    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G33" s="3">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="H33" s="11">
+        <f t="shared" si="8"/>
+        <v>70.391375464684018</v>
+      </c>
+      <c r="I33" s="11">
+        <f t="shared" si="9"/>
+        <v>66.493234200743501</v>
+      </c>
+      <c r="J33" s="11">
+        <f t="shared" si="10"/>
+        <v>40.514855018587355</v>
+      </c>
+      <c r="L33" s="3">
+        <v>20</v>
+      </c>
+      <c r="M33" s="20">
+        <f t="shared" si="12"/>
+        <v>72.862453531598518</v>
+      </c>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4">
+        <f>L48</f>
+        <v>49</v>
+      </c>
+      <c r="P33" s="20">
+        <f>AVERAGE(M48:M50)</f>
+        <v>69.219330855018583</v>
+      </c>
+      <c r="Q33" s="20">
+        <f>_xlfn.STDEV.S(M48:M50)</f>
+        <v>0.52044609665427544</v>
+      </c>
+      <c r="R33" s="22">
+        <f t="shared" si="13"/>
+        <v>0.75187969924812081</v>
+      </c>
+      <c r="S33" s="20">
+        <f t="shared" si="14"/>
+        <v>70.780669144981402</v>
+      </c>
+      <c r="T33" s="14">
+        <f>P33-Q33*3</f>
+        <v>67.657992565055764</v>
+      </c>
+    </row>
+    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G34" s="3">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="H34" s="11">
+        <f t="shared" si="8"/>
+        <v>70.908959107806695</v>
+      </c>
+      <c r="I34" s="11">
+        <f t="shared" si="9"/>
+        <v>67.64508550185873</v>
+      </c>
+      <c r="J34" s="11">
+        <f t="shared" si="10"/>
+        <v>38.727434944237913</v>
+      </c>
+      <c r="L34" s="3">
+        <v>20</v>
+      </c>
+      <c r="M34" s="20">
+        <f t="shared" si="12"/>
+        <v>72.862453531598518</v>
+      </c>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G35" s="3">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="H35" s="11">
+        <f t="shared" si="8"/>
+        <v>70.287858736059491</v>
+      </c>
+      <c r="I35" s="11">
+        <f t="shared" si="9"/>
+        <v>67.854513011152406</v>
+      </c>
+      <c r="J35" s="11">
+        <f t="shared" si="10"/>
+        <v>38.727434944237913</v>
+      </c>
+      <c r="L35" s="3">
+        <v>20</v>
+      </c>
+      <c r="M35" s="20">
+        <f t="shared" si="12"/>
+        <v>72.862453531598518</v>
+      </c>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="5"/>
+    </row>
+    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G36" s="3">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="H36" s="11">
+        <f t="shared" si="8"/>
+        <v>70.598408921933085</v>
+      </c>
+      <c r="I36" s="11">
+        <f>I18*$C$23*$C$28</f>
+        <v>67.854513011152406</v>
+      </c>
+      <c r="J36" s="11">
+        <f t="shared" si="10"/>
+        <v>39.720446096654271</v>
+      </c>
+      <c r="L36" s="3">
+        <v>20</v>
+      </c>
+      <c r="M36" s="20">
+        <f t="shared" si="12"/>
+        <v>72.862453531598518</v>
+      </c>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4">
+        <f>INTERCEPT(P29:P33,O29:O33)</f>
+        <v>75.393923391227361</v>
+      </c>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="5"/>
+    </row>
+    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G37" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="11">
+        <f>AVERAGE(H27:H36)</f>
+        <v>70.65047514268737</v>
+      </c>
+      <c r="I37" s="11">
+        <f>AVERAGE(I27:I36)</f>
+        <v>67.45660074349442</v>
+      </c>
+      <c r="J37" s="13">
+        <f>AVERAGE(J27:J36)</f>
+        <v>39.859467657992568</v>
+      </c>
+      <c r="L37" s="3">
+        <v>20</v>
+      </c>
+      <c r="M37" s="20">
+        <f t="shared" si="12"/>
+        <v>72.862453531598518</v>
+      </c>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4">
+        <f>SLOPE(P29:P33,O29:O33)</f>
+        <v>-0.1225546645273568</v>
+      </c>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="5"/>
+    </row>
+    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="4">
+        <f>_xlfn.STDEV.S(H27:H36)</f>
+        <v>0.31403474207477416</v>
+      </c>
+      <c r="I38" s="4">
+        <f>_xlfn.STDEV.S(I27:I36)</f>
+        <v>0.5402886996548264</v>
+      </c>
+      <c r="J38" s="5">
+        <f>_xlfn.STDEV.S(J27:J36)</f>
+        <v>0.85831504217970955</v>
+      </c>
+      <c r="L38" s="3">
+        <v>20</v>
+      </c>
+      <c r="M38" s="20">
+        <f t="shared" si="12"/>
+        <v>72.862453531598518</v>
+      </c>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="5"/>
+    </row>
+    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G39" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="11">
+        <f>H37+3*H38</f>
+        <v>71.592579368911686</v>
+      </c>
+      <c r="I39" s="11">
+        <f t="shared" ref="I39:J39" si="16">I37+3*I38</f>
+        <v>69.077466842458904</v>
+      </c>
+      <c r="J39" s="13">
+        <f t="shared" si="16"/>
+        <v>42.434412784531695</v>
+      </c>
+      <c r="L39" s="3">
+        <v>30</v>
+      </c>
+      <c r="M39" s="20">
+        <f t="shared" si="12"/>
+        <v>71.821561338289968</v>
+      </c>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="5"/>
+    </row>
+    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G40" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="11">
+        <f>H37-3*H38</f>
+        <v>69.708370916463053</v>
+      </c>
+      <c r="I40" s="11">
+        <f t="shared" ref="I40:J40" si="17">I37-3*I38</f>
+        <v>65.835734644529936</v>
+      </c>
+      <c r="J40" s="13">
+        <f t="shared" si="17"/>
+        <v>37.28452253145344</v>
+      </c>
+      <c r="L40" s="3">
+        <v>30</v>
+      </c>
+      <c r="M40" s="20">
+        <f t="shared" si="12"/>
+        <v>71.821561338289968</v>
+      </c>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="5"/>
+    </row>
+    <row r="41" spans="7:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="7">
+        <f>H38/H37*100</f>
+        <v>0.44449063002130162</v>
+      </c>
+      <c r="I41" s="7">
+        <f>I38/I37*100</f>
+        <v>0.8009426708429751</v>
+      </c>
+      <c r="J41" s="8">
+        <f>J38/J37*100</f>
+        <v>2.1533529989520606</v>
+      </c>
+      <c r="L41" s="3">
+        <v>30</v>
+      </c>
+      <c r="M41" s="20">
+        <f t="shared" si="12"/>
+        <v>71.821561338289968</v>
+      </c>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="5"/>
+    </row>
+    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="L42" s="3">
+        <v>35</v>
+      </c>
+      <c r="M42" s="20">
+        <f t="shared" si="12"/>
+        <v>70.988847583643121</v>
+      </c>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="5"/>
+    </row>
+    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="L43" s="3">
+        <v>35</v>
+      </c>
+      <c r="M43" s="20">
+        <f t="shared" si="12"/>
+        <v>71.19702602230484</v>
+      </c>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="5"/>
+    </row>
+    <row r="44" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="L44" s="3">
+        <v>35</v>
+      </c>
+      <c r="M44" s="20">
+        <f t="shared" si="12"/>
+        <v>71.301115241635685</v>
+      </c>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="5"/>
+    </row>
+    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="L45" s="3">
+        <v>40</v>
+      </c>
+      <c r="M45" s="20">
+        <f t="shared" si="12"/>
+        <v>70.572490706319698</v>
+      </c>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="5"/>
+    </row>
+    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="L46" s="3">
+        <v>40</v>
+      </c>
+      <c r="M46" s="20">
+        <f t="shared" si="12"/>
+        <v>70.572490706319698</v>
+      </c>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="5"/>
+    </row>
+    <row r="47" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="L47" s="3">
+        <v>40</v>
+      </c>
+      <c r="M47" s="20">
+        <f t="shared" si="12"/>
+        <v>70.780669144981417</v>
+      </c>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="5"/>
+    </row>
+    <row r="48" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="L48" s="3">
+        <v>49</v>
+      </c>
+      <c r="M48" s="20">
+        <f>M23*$C$23</f>
+        <v>68.698884758364315</v>
+      </c>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="5"/>
+    </row>
+    <row r="49" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="L49" s="3">
+        <v>49</v>
+      </c>
+      <c r="M49" s="20">
+        <f t="shared" si="12"/>
+        <v>69.219330855018583</v>
+      </c>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="5"/>
+    </row>
+    <row r="50" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L50" s="6">
+        <v>49</v>
+      </c>
+      <c r="M50" s="20">
+        <f t="shared" si="12"/>
+        <v>69.739776951672866</v>
+      </c>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="8"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M4:M13">
     <sortCondition ref="M4"/>
   </sortState>
   <conditionalFormatting sqref="H9:H18">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+      <formula>$H$19-$H$20*3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+      <formula>$H$19+$H$20*3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:H36">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>$H$37-$H$38*3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>$H$37+$H$38*3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4967E49E-EFE3-4D15-A052-22D31E5679B2}">
+  <dimension ref="B2:K24"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4">
+        <v>69.8</v>
+      </c>
+      <c r="D3">
+        <v>72.6542750929368</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>72.8</v>
+      </c>
+      <c r="H3">
+        <v>8.777573678782484E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.12057106701624293</v>
+      </c>
+      <c r="J3">
+        <v>73.063327210363468</v>
+      </c>
+      <c r="K3">
+        <v>72.536672789636526</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4">
+        <v>69.8</v>
+      </c>
+      <c r="D4">
+        <v>72.6542750929368</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>71.821561338289968</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>71.821561338289968</v>
+      </c>
+      <c r="K4">
+        <v>71.821561338289968</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="D5">
+        <v>72.758364312267659</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>71.162329615861211</v>
+      </c>
+      <c r="H5">
+        <v>0.15899890887083501</v>
+      </c>
+      <c r="I5">
+        <v>0.22343128693105083</v>
+      </c>
+      <c r="J5">
+        <v>71.639326342473709</v>
+      </c>
+      <c r="K5">
+        <v>70.685332889248713</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="D6">
+        <v>72.758364312267659</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>70.641883519206942</v>
+      </c>
+      <c r="H6">
+        <v>0.12019187760081929</v>
+      </c>
+      <c r="I6">
+        <v>0.17014251547828579</v>
+      </c>
+      <c r="J6">
+        <v>71.002459152009394</v>
+      </c>
+      <c r="K6">
+        <v>70.281307886404491</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4">
+        <v>70</v>
+      </c>
+      <c r="D7">
+        <v>72.862453531598518</v>
+      </c>
+      <c r="F7">
+        <v>49</v>
+      </c>
+      <c r="G7">
+        <v>69.219330855018583</v>
+      </c>
+      <c r="H7">
+        <v>0.52044609665427544</v>
+      </c>
+      <c r="I7">
+        <v>0.75187969924812081</v>
+      </c>
+      <c r="J7">
+        <v>70.780669144981402</v>
+      </c>
+      <c r="K7">
+        <v>67.657992565055764</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4">
+        <v>70</v>
+      </c>
+      <c r="D8">
+        <v>72.862453531598518</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4">
+        <v>70</v>
+      </c>
+      <c r="D9">
+        <v>72.862453531598518</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4">
+        <v>70</v>
+      </c>
+      <c r="D10">
+        <v>72.862453531598518</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4">
+        <v>70</v>
+      </c>
+      <c r="D11">
+        <v>72.862453531598518</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4">
+        <v>70</v>
+      </c>
+      <c r="D12">
+        <v>72.862453531598518</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4">
+        <v>69</v>
+      </c>
+      <c r="D13">
+        <v>71.821561338289968</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>30</v>
+      </c>
+      <c r="C14" s="4">
+        <v>69</v>
+      </c>
+      <c r="D14">
+        <v>71.821561338289968</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>71.821561338289968</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4">
+        <v>68.2</v>
+      </c>
+      <c r="D16">
+        <v>70.988847583643121</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="D17">
+        <v>71.19702602230484</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4">
+        <v>68.5</v>
+      </c>
+      <c r="D18">
+        <v>71.301115241635685</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>40</v>
+      </c>
+      <c r="C19" s="4">
+        <v>67.8</v>
+      </c>
+      <c r="D19">
+        <v>70.572490706319698</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>40</v>
+      </c>
+      <c r="C20" s="4">
+        <v>67.8</v>
+      </c>
+      <c r="D20">
+        <v>70.572490706319698</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>40</v>
+      </c>
+      <c r="C21" s="4">
+        <v>68</v>
+      </c>
+      <c r="D21">
+        <v>70.780669144981417</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>49</v>
+      </c>
+      <c r="C22" s="4">
+        <v>66</v>
+      </c>
+      <c r="D22">
+        <v>68.698884758364315</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>49</v>
+      </c>
+      <c r="C23" s="4">
+        <v>66.5</v>
+      </c>
+      <c r="D23">
+        <v>69.219330855018583</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="6">
+        <v>49</v>
+      </c>
+      <c r="C24" s="7">
+        <v>67</v>
+      </c>
+      <c r="D24">
+        <v>69.739776951672866</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E2010C-5649-40B0-AF60-C9728FAC25B9}">
+  <dimension ref="A3:P24"/>
+  <sheetViews>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="C3" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="26">
+        <v>1</v>
+      </c>
+      <c r="D4" s="27">
+        <v>68.80297397769516</v>
+      </c>
+      <c r="E4" s="24">
+        <v>71.222587858100354</v>
+      </c>
+      <c r="F4" s="27">
+        <v>65</v>
+      </c>
+      <c r="G4" s="24">
+        <v>68.063940520446096</v>
+      </c>
+      <c r="H4" s="27">
+        <v>39</v>
+      </c>
+      <c r="I4" s="24">
+        <v>38.727434944237913</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="26">
+        <v>2</v>
+      </c>
+      <c r="D5" s="27">
+        <v>68</v>
+      </c>
+      <c r="E5" s="24">
+        <v>70.391375464684018</v>
+      </c>
+      <c r="F5" s="27">
+        <v>64.5</v>
+      </c>
+      <c r="G5" s="24">
+        <v>67.540371747211893</v>
+      </c>
+      <c r="H5" s="27">
+        <v>40</v>
+      </c>
+      <c r="I5" s="24">
+        <v>39.720446096654271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="26">
+        <v>3</v>
+      </c>
+      <c r="D6" s="27">
+        <v>68.5</v>
+      </c>
+      <c r="E6" s="24">
+        <v>70.908959107806695</v>
+      </c>
+      <c r="F6" s="27">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="G6" s="24">
+        <v>67.435657992565055</v>
+      </c>
+      <c r="H6" s="27">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="I6" s="24">
+        <v>40.514855018587355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="26">
+        <v>4</v>
+      </c>
+      <c r="D7" s="27">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="E7" s="24">
+        <v>70.494892193308544</v>
+      </c>
+      <c r="F7" s="27">
+        <v>63.5</v>
+      </c>
+      <c r="G7" s="24">
+        <v>66.493234200743501</v>
+      </c>
+      <c r="H7" s="27">
+        <v>41</v>
+      </c>
+      <c r="I7" s="24">
+        <v>40.713457249070629</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="26">
+        <v>5</v>
+      </c>
+      <c r="D8" s="27">
+        <v>68.5</v>
+      </c>
+      <c r="E8" s="24">
+        <v>70.908959107806695</v>
+      </c>
+      <c r="F8" s="27">
+        <v>64.5</v>
+      </c>
+      <c r="G8" s="24">
+        <v>67.540371747211893</v>
+      </c>
+      <c r="H8" s="27">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="I8" s="24">
+        <v>40.514855018587355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="26">
+        <v>6</v>
+      </c>
+      <c r="D9" s="27">
+        <v>68</v>
+      </c>
+      <c r="E9" s="24">
+        <v>70.391375464684018</v>
+      </c>
+      <c r="F9" s="27">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="G9" s="24">
+        <v>67.64508550185873</v>
+      </c>
+      <c r="H9" s="27">
+        <v>41</v>
+      </c>
+      <c r="I9" s="24">
+        <v>40.713457249070629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="26">
+        <v>7</v>
+      </c>
+      <c r="D10" s="27">
+        <v>68</v>
+      </c>
+      <c r="E10" s="24">
+        <v>70.391375464684018</v>
+      </c>
+      <c r="F10" s="27">
+        <v>63.5</v>
+      </c>
+      <c r="G10" s="24">
+        <v>66.493234200743501</v>
+      </c>
+      <c r="H10" s="27">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="I10" s="24">
+        <v>40.514855018587355</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="26">
+        <v>8</v>
+      </c>
+      <c r="D11" s="27">
+        <v>68.5</v>
+      </c>
+      <c r="E11" s="24">
+        <v>70.908959107806695</v>
+      </c>
+      <c r="F11" s="27">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="G11" s="24">
+        <v>67.64508550185873</v>
+      </c>
+      <c r="H11" s="27">
+        <v>39</v>
+      </c>
+      <c r="I11" s="24">
+        <v>38.727434944237913</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="26">
+        <v>9</v>
+      </c>
+      <c r="D12" s="27">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="E12" s="24">
+        <v>70.287858736059491</v>
+      </c>
+      <c r="F12" s="27">
+        <v>64.8</v>
+      </c>
+      <c r="G12" s="24">
+        <v>67.854513011152406</v>
+      </c>
+      <c r="H12" s="27">
+        <v>39</v>
+      </c>
+      <c r="I12" s="24">
+        <v>38.727434944237913</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="26">
+        <v>10</v>
+      </c>
+      <c r="D13" s="27">
+        <v>68.2</v>
+      </c>
+      <c r="E13" s="24">
+        <v>70.598408921933085</v>
+      </c>
+      <c r="F13" s="27">
+        <v>64.8</v>
+      </c>
+      <c r="G13" s="24">
+        <v>67.854513011152406</v>
+      </c>
+      <c r="H13" s="27">
+        <v>40</v>
+      </c>
+      <c r="I13" s="24">
+        <v>39.720446096654271</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="27">
+        <f>AVERAGE(D4:D13)</f>
+        <v>68.250297397769515</v>
+      </c>
+      <c r="E14" s="27">
+        <f t="shared" ref="E14:I14" si="0">AVERAGE(E4:E13)</f>
+        <v>70.65047514268737</v>
+      </c>
+      <c r="F14" s="27">
+        <f t="shared" si="0"/>
+        <v>64.419999999999987</v>
+      </c>
+      <c r="G14" s="27">
+        <f t="shared" si="0"/>
+        <v>67.45660074349442</v>
+      </c>
+      <c r="H14" s="27">
+        <f t="shared" si="0"/>
+        <v>40.14</v>
+      </c>
+      <c r="I14" s="27">
+        <f t="shared" si="0"/>
+        <v>39.859467657992568</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24">
+        <v>0.31403474207477416</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24">
+        <v>0.5402886996548264</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24">
+        <v>0.85831504217970955</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24">
+        <v>71.592579368911686</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24">
+        <v>69.077466842458904</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24">
+        <v>42.434412784531695</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24">
+        <v>69.708370916463053</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24">
+        <v>65.835734644529936</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24">
+        <v>37.28452253145344</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24">
+        <v>0.44449063002130162</v>
+      </c>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24">
+        <v>0.8009426708429751</v>
+      </c>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24">
+        <v>2.1533529989520601</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="28"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="23">
+        <v>1</v>
+      </c>
+      <c r="E22" s="24">
+        <f>D14</f>
+        <v>68.250297397769515</v>
+      </c>
+      <c r="F22">
+        <f>'Daten SURF'!C27</f>
+        <v>0.99450000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>0.8</v>
+      </c>
+      <c r="E23" s="24">
+        <f>F14</f>
+        <v>64.419999999999987</v>
+      </c>
+      <c r="F23">
+        <f>'Daten SURF'!C28</f>
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="24">
+        <f>H14</f>
+        <v>40.14</v>
+      </c>
+      <c r="F24">
+        <f>'Daten SURF'!C29</f>
+        <v>0.95399999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J3:K3">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>$H$19-$H$20*3</formula>
     </cfRule>

</xml_diff>